<commit_message>
update doc and tables after testing on fpga
</commit_message>
<xml_diff>
--- a/Mips_Pipeline_Test.xlsx
+++ b/Mips_Pipeline_Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CTI_3rd_year_1\Structure_of_Computer_Systems\SCS-Assignment-Pipeline-MIPS-CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B458508E-140C-4052-9CE8-80B5968CF4D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B02CC8-D7B2-416A-90A7-99914D810D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{AE386CA4-EDC2-4F06-A869-52A3BC7A21B9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AE386CA4-EDC2-4F06-A869-52A3BC7A21B9}"/>
   </bookViews>
   <sheets>
     <sheet name="instruction_exec" sheetId="1" r:id="rId1"/>
@@ -3551,8 +3551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2326B967-B418-496E-AAA0-FF8CE45CE59E}">
   <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3847,10 +3847,10 @@
       <c r="R5" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S5" s="33" t="s">
+      <c r="S5" s="42" t="s">
         <v>180</v>
       </c>
-      <c r="T5" s="33" t="s">
+      <c r="T5" s="42" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3909,11 +3909,11 @@
       <c r="R6" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S6" s="42" t="s">
-        <v>180</v>
-      </c>
-      <c r="T6" s="42" t="s">
-        <v>180</v>
+      <c r="S6" s="56" t="s">
+        <v>206</v>
+      </c>
+      <c r="T6" s="56" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
@@ -3971,11 +3971,11 @@
       <c r="R7" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S7" s="56" t="s">
-        <v>206</v>
-      </c>
-      <c r="T7" s="56" t="s">
-        <v>195</v>
+      <c r="S7" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="T7" s="41" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
@@ -4033,11 +4033,11 @@
       <c r="R8" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S8" s="41" t="s">
-        <v>238</v>
-      </c>
-      <c r="T8" s="41" t="s">
-        <v>210</v>
+      <c r="S8" s="62" t="s">
+        <v>250</v>
+      </c>
+      <c r="T8" s="62" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
@@ -4095,10 +4095,10 @@
       <c r="R9" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S9" s="62" t="s">
+      <c r="S9" s="63" t="s">
         <v>240</v>
       </c>
-      <c r="T9" s="62" t="s">
+      <c r="T9" s="63" t="s">
         <v>197</v>
       </c>
     </row>
@@ -4157,10 +4157,10 @@
       <c r="R10" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S10" s="63" t="s">
+      <c r="S10" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="T10" s="63" t="s">
+      <c r="T10" s="42" t="s">
         <v>196</v>
       </c>
     </row>
@@ -4219,10 +4219,10 @@
       <c r="R11" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S11" s="42" t="s">
+      <c r="S11" s="56" t="s">
         <v>236</v>
       </c>
-      <c r="T11" s="42" t="s">
+      <c r="T11" s="56" t="s">
         <v>199</v>
       </c>
     </row>
@@ -4281,10 +4281,10 @@
       <c r="R12" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S12" s="56" t="s">
+      <c r="S12" s="41" t="s">
         <v>250</v>
       </c>
-      <c r="T12" s="56" t="s">
+      <c r="T12" s="41" t="s">
         <v>198</v>
       </c>
     </row>
@@ -4343,10 +4343,10 @@
       <c r="R13" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S13" s="41" t="s">
+      <c r="S13" s="62" t="s">
         <v>200</v>
       </c>
-      <c r="T13" s="41" t="s">
+      <c r="T13" s="62" t="s">
         <v>180</v>
       </c>
     </row>
@@ -4405,10 +4405,10 @@
       <c r="R14" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S14" s="62" t="s">
+      <c r="S14" s="63" t="s">
         <v>210</v>
       </c>
-      <c r="T14" s="62" t="s">
+      <c r="T14" s="63" t="s">
         <v>278</v>
       </c>
     </row>
@@ -4467,10 +4467,10 @@
       <c r="R15" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S15" s="63" t="s">
+      <c r="S15" s="42" t="s">
         <v>265</v>
       </c>
-      <c r="T15" s="63" t="s">
+      <c r="T15" s="42" t="s">
         <v>194</v>
       </c>
     </row>
@@ -4529,10 +4529,10 @@
       <c r="R16" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S16" s="42" t="s">
+      <c r="S16" s="56" t="s">
         <v>193</v>
       </c>
-      <c r="T16" s="42" t="s">
+      <c r="T16" s="56" t="s">
         <v>181</v>
       </c>
     </row>
@@ -4591,10 +4591,10 @@
       <c r="R17" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S17" s="56" t="s">
+      <c r="S17" s="41" t="s">
         <v>236</v>
       </c>
-      <c r="T17" s="56" t="s">
+      <c r="T17" s="41" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4653,10 +4653,10 @@
       <c r="R18" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S18" s="41" t="s">
+      <c r="S18" s="62" t="s">
         <v>250</v>
       </c>
-      <c r="T18" s="41" t="s">
+      <c r="T18" s="62" t="s">
         <v>200</v>
       </c>
     </row>
@@ -4715,10 +4715,10 @@
       <c r="R19" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S19" s="62" t="s">
+      <c r="S19" s="63" t="s">
         <v>210</v>
       </c>
-      <c r="T19" s="62" t="s">
+      <c r="T19" s="63" t="s">
         <v>279</v>
       </c>
     </row>
@@ -4777,10 +4777,10 @@
       <c r="R20" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S20" s="63" t="s">
+      <c r="S20" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="T20" s="63" t="s">
+      <c r="T20" s="42" t="s">
         <v>202</v>
       </c>
     </row>
@@ -4839,10 +4839,10 @@
       <c r="R21" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S21" s="42" t="s">
+      <c r="S21" s="56" t="s">
         <v>210</v>
       </c>
-      <c r="T21" s="42" t="s">
+      <c r="T21" s="56" t="s">
         <v>203</v>
       </c>
     </row>
@@ -4901,10 +4901,10 @@
       <c r="R22" s="33" t="s">
         <v>245</v>
       </c>
-      <c r="S22" s="56" t="s">
+      <c r="S22" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="T22" s="56" t="s">
+      <c r="T22" s="41" t="s">
         <v>283</v>
       </c>
     </row>
@@ -5542,10 +5542,10 @@
       <c r="O33" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S33" s="41" t="s">
+      <c r="S33" s="42" t="s">
         <v>284</v>
       </c>
-      <c r="T33" s="41" t="s">
+      <c r="T33" s="42" t="s">
         <v>284</v>
       </c>
     </row>
@@ -6005,10 +6005,10 @@
       <c r="R41" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="S41" s="42" t="s">
+      <c r="S41" s="63" t="s">
         <v>284</v>
       </c>
-      <c r="T41" s="42" t="s">
+      <c r="T41" s="63" t="s">
         <v>285</v>
       </c>
     </row>
@@ -6241,10 +6241,10 @@
       <c r="R45" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="S45" s="62" t="s">
+      <c r="S45" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="T45" s="62" t="s">
+      <c r="T45" s="41" t="s">
         <v>286</v>
       </c>
     </row>
@@ -6305,8 +6305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3B9EAD-36F4-4B74-8350-B30B3341E79E}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6316,7 +6316,7 @@
     <col min="3" max="3" width="13.81640625" customWidth="1"/>
     <col min="4" max="4" width="7.90625" customWidth="1"/>
     <col min="5" max="5" width="9.26953125" customWidth="1"/>
-    <col min="11" max="11" width="12.54296875" customWidth="1"/>
+    <col min="13" max="13" width="12.54296875" customWidth="1"/>
     <col min="15" max="15" width="9.6328125" customWidth="1"/>
     <col min="16" max="16" width="11.08984375" customWidth="1"/>
     <col min="20" max="20" width="11.6328125" customWidth="1"/>
@@ -6367,10 +6367,10 @@
       <c r="L2" s="88"/>
       <c r="M2" s="88"/>
       <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="89" t="s">
+      <c r="O2" s="89" t="s">
         <v>92</v>
       </c>
+      <c r="P2" s="89"/>
       <c r="Q2" s="89"/>
       <c r="R2" s="89"/>
       <c r="S2" s="91" t="s">
@@ -6402,27 +6402,27 @@
         <v>94</v>
       </c>
       <c r="H3" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="20" t="s">
         <v>96</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>95</v>
       </c>
       <c r="J3" s="68" t="s">
         <v>97</v>
       </c>
       <c r="K3" s="34" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="L3" s="34" t="s">
         <v>99</v>
       </c>
       <c r="M3" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="N3" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="N3" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="O3" s="34" t="s">
+      <c r="O3" s="69" t="s">
         <v>189</v>
       </c>
       <c r="P3" s="69" t="s">
@@ -6475,17 +6475,17 @@
       <c r="J4" s="19">
         <v>0</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="78">
+        <v>1</v>
+      </c>
+      <c r="L4" s="19">
+        <v>0</v>
+      </c>
+      <c r="M4" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L4" s="19">
-        <v>0</v>
-      </c>
-      <c r="M4" s="19">
-        <v>0</v>
-      </c>
-      <c r="N4" s="78">
-        <v>1</v>
+      <c r="N4" s="19">
+        <v>0</v>
       </c>
       <c r="O4" s="19">
         <v>0</v>
@@ -6540,17 +6540,17 @@
       <c r="J5" s="19">
         <v>0</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="78">
+        <v>1</v>
+      </c>
+      <c r="L5" s="19">
+        <v>0</v>
+      </c>
+      <c r="M5" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="L5" s="19">
-        <v>0</v>
-      </c>
-      <c r="M5" s="19">
-        <v>0</v>
-      </c>
-      <c r="N5" s="78">
-        <v>1</v>
+      <c r="N5" s="19">
+        <v>0</v>
       </c>
       <c r="O5" s="19">
         <v>0</v>
@@ -6605,14 +6605,14 @@
       <c r="J6" s="72">
         <v>1</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="19">
+        <v>0</v>
+      </c>
+      <c r="L6" s="78">
+        <v>1</v>
+      </c>
+      <c r="M6" s="19" t="s">
         <v>207</v>
-      </c>
-      <c r="L6" s="78">
-        <v>1</v>
-      </c>
-      <c r="M6" s="19">
-        <v>0</v>
       </c>
       <c r="N6" s="19">
         <v>0</v>
@@ -6670,17 +6670,17 @@
       <c r="J7" s="19">
         <v>0</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="78">
+        <v>1</v>
+      </c>
+      <c r="L7" s="19">
+        <v>0</v>
+      </c>
+      <c r="M7" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="L7" s="19">
-        <v>0</v>
-      </c>
-      <c r="M7" s="19">
-        <v>0</v>
-      </c>
-      <c r="N7" s="78">
-        <v>1</v>
+      <c r="N7" s="19">
+        <v>0</v>
       </c>
       <c r="O7" s="19">
         <v>0</v>
@@ -6735,14 +6735,14 @@
       <c r="J8" s="72">
         <v>1</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="19">
+        <v>0</v>
+      </c>
+      <c r="L8" s="78">
+        <v>1</v>
+      </c>
+      <c r="M8" s="19" t="s">
         <v>207</v>
-      </c>
-      <c r="L8" s="78">
-        <v>1</v>
-      </c>
-      <c r="M8" s="19">
-        <v>0</v>
       </c>
       <c r="N8" s="19">
         <v>0</v>
@@ -6800,17 +6800,17 @@
       <c r="J9" s="72">
         <v>1</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="78">
+        <v>1</v>
+      </c>
+      <c r="L9" s="78">
+        <v>1</v>
+      </c>
+      <c r="M9" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="L9" s="78">
-        <v>1</v>
-      </c>
-      <c r="M9" s="19">
-        <v>0</v>
-      </c>
-      <c r="N9" s="78">
-        <v>1</v>
+      <c r="N9" s="19">
+        <v>0</v>
       </c>
       <c r="O9" s="19">
         <v>1</v>
@@ -6865,17 +6865,17 @@
       <c r="J10" s="72">
         <v>1</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="78">
+        <v>1</v>
+      </c>
+      <c r="L10" s="78">
+        <v>1</v>
+      </c>
+      <c r="M10" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="L10" s="78">
-        <v>1</v>
-      </c>
-      <c r="M10" s="19">
-        <v>0</v>
-      </c>
-      <c r="N10" s="78">
-        <v>1</v>
+      <c r="N10" s="19">
+        <v>0</v>
       </c>
       <c r="O10" s="19">
         <v>1</v>
@@ -6930,14 +6930,14 @@
       <c r="J11" s="19">
         <v>0</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="K11" s="78">
+        <v>1</v>
+      </c>
+      <c r="L11" s="19">
+        <v>0</v>
+      </c>
+      <c r="M11" s="19" t="s">
         <v>289</v>
-      </c>
-      <c r="L11" s="19">
-        <v>0</v>
-      </c>
-      <c r="M11" s="78">
-        <v>1</v>
       </c>
       <c r="N11" s="78">
         <v>1</v>
@@ -6995,14 +6995,14 @@
       <c r="J12" s="19">
         <v>0</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="78">
+        <v>1</v>
+      </c>
+      <c r="L12" s="19">
+        <v>0</v>
+      </c>
+      <c r="M12" s="19" t="s">
         <v>290</v>
-      </c>
-      <c r="L12" s="19">
-        <v>0</v>
-      </c>
-      <c r="M12" s="78">
-        <v>1</v>
       </c>
       <c r="N12" s="78">
         <v>1</v>
@@ -7060,14 +7060,14 @@
       <c r="J13" s="72">
         <v>1</v>
       </c>
-      <c r="K13" s="19" t="s">
+      <c r="K13" s="19">
+        <v>0</v>
+      </c>
+      <c r="L13" s="78">
+        <v>1</v>
+      </c>
+      <c r="M13" s="19" t="s">
         <v>289</v>
-      </c>
-      <c r="L13" s="78">
-        <v>1</v>
-      </c>
-      <c r="M13" s="19">
-        <v>0</v>
       </c>
       <c r="N13" s="19">
         <v>0</v>
@@ -7125,17 +7125,17 @@
       <c r="J14" s="19">
         <v>0</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="78">
+        <v>1</v>
+      </c>
+      <c r="L14" s="19">
+        <v>0</v>
+      </c>
+      <c r="M14" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="L14" s="19">
-        <v>0</v>
-      </c>
-      <c r="M14" s="19">
-        <v>0</v>
-      </c>
-      <c r="N14" s="78">
-        <v>1</v>
+      <c r="N14" s="19">
+        <v>0</v>
       </c>
       <c r="O14" s="19">
         <v>0</v>
@@ -7190,14 +7190,14 @@
       <c r="J15" s="72">
         <v>1</v>
       </c>
-      <c r="K15" s="19" t="s">
+      <c r="K15" s="19">
+        <v>0</v>
+      </c>
+      <c r="L15" s="78">
+        <v>1</v>
+      </c>
+      <c r="M15" s="19" t="s">
         <v>207</v>
-      </c>
-      <c r="L15" s="78">
-        <v>1</v>
-      </c>
-      <c r="M15" s="19">
-        <v>0</v>
       </c>
       <c r="N15" s="19">
         <v>0</v>
@@ -7255,14 +7255,14 @@
       <c r="J16" s="72">
         <v>1</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="19">
+        <v>0</v>
+      </c>
+      <c r="L16" s="78">
+        <v>1</v>
+      </c>
+      <c r="M16" s="19" t="s">
         <v>188</v>
-      </c>
-      <c r="L16" s="78">
-        <v>1</v>
-      </c>
-      <c r="M16" s="19">
-        <v>0</v>
       </c>
       <c r="N16" s="19">
         <v>0</v>
@@ -7320,14 +7320,14 @@
       <c r="J17" s="72">
         <v>1</v>
       </c>
-      <c r="K17" s="19" t="s">
+      <c r="K17" s="19">
+        <v>0</v>
+      </c>
+      <c r="L17" s="78">
+        <v>1</v>
+      </c>
+      <c r="M17" s="19" t="s">
         <v>207</v>
-      </c>
-      <c r="L17" s="78">
-        <v>1</v>
-      </c>
-      <c r="M17" s="19">
-        <v>0</v>
       </c>
       <c r="N17" s="19">
         <v>0</v>
@@ -7385,14 +7385,14 @@
       <c r="J18" s="72">
         <v>1</v>
       </c>
-      <c r="K18" s="19" t="s">
+      <c r="K18" s="19">
+        <v>0</v>
+      </c>
+      <c r="L18" s="78">
+        <v>1</v>
+      </c>
+      <c r="M18" s="19" t="s">
         <v>207</v>
-      </c>
-      <c r="L18" s="78">
-        <v>1</v>
-      </c>
-      <c r="M18" s="19">
-        <v>0</v>
       </c>
       <c r="N18" s="19">
         <v>0</v>
@@ -7450,17 +7450,17 @@
       <c r="J19" s="19">
         <v>0</v>
       </c>
-      <c r="K19" s="19" t="s">
+      <c r="K19" s="78">
+        <v>1</v>
+      </c>
+      <c r="L19" s="19">
+        <v>0</v>
+      </c>
+      <c r="M19" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="L19" s="19">
-        <v>0</v>
-      </c>
-      <c r="M19" s="19">
-        <v>0</v>
-      </c>
-      <c r="N19" s="78">
-        <v>1</v>
+      <c r="N19" s="19">
+        <v>0</v>
       </c>
       <c r="O19" s="19">
         <v>0</v>
@@ -7515,17 +7515,17 @@
       <c r="J20" s="19">
         <v>0</v>
       </c>
-      <c r="K20" s="19" t="s">
+      <c r="K20" s="78">
+        <v>1</v>
+      </c>
+      <c r="L20" s="19">
+        <v>0</v>
+      </c>
+      <c r="M20" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="L20" s="19">
-        <v>0</v>
-      </c>
-      <c r="M20" s="19">
-        <v>0</v>
-      </c>
-      <c r="N20" s="78">
-        <v>1</v>
+      <c r="N20" s="19">
+        <v>0</v>
       </c>
       <c r="O20" s="19">
         <v>0</v>
@@ -7580,17 +7580,17 @@
       <c r="J21" s="72">
         <v>1</v>
       </c>
-      <c r="K21" s="19" t="s">
+      <c r="K21" s="78">
+        <v>1</v>
+      </c>
+      <c r="L21" s="78">
+        <v>1</v>
+      </c>
+      <c r="M21" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="L21" s="78">
-        <v>1</v>
-      </c>
-      <c r="M21" s="19">
-        <v>0</v>
-      </c>
-      <c r="N21" s="78">
-        <v>1</v>
+      <c r="N21" s="19">
+        <v>0</v>
       </c>
       <c r="O21" s="19">
         <v>0</v>
@@ -7645,14 +7645,14 @@
       <c r="J22" s="72">
         <v>1</v>
       </c>
-      <c r="K22" s="19" t="s">
+      <c r="K22" s="19">
+        <v>0</v>
+      </c>
+      <c r="L22" s="78">
+        <v>1</v>
+      </c>
+      <c r="M22" s="19" t="s">
         <v>294</v>
-      </c>
-      <c r="L22" s="78">
-        <v>1</v>
-      </c>
-      <c r="M22" s="19">
-        <v>0</v>
       </c>
       <c r="N22" s="19">
         <v>0</v>
@@ -7710,14 +7710,14 @@
       <c r="J23" s="72">
         <v>1</v>
       </c>
-      <c r="K23" s="19" t="s">
+      <c r="K23" s="19">
+        <v>0</v>
+      </c>
+      <c r="L23" s="78">
+        <v>1</v>
+      </c>
+      <c r="M23" s="19" t="s">
         <v>207</v>
-      </c>
-      <c r="L23" s="78">
-        <v>1</v>
-      </c>
-      <c r="M23" s="19">
-        <v>0</v>
       </c>
       <c r="N23" s="19">
         <v>0</v>
@@ -7775,14 +7775,14 @@
       <c r="J24" s="72">
         <v>1</v>
       </c>
-      <c r="K24" s="19" t="s">
+      <c r="K24" s="19">
+        <v>0</v>
+      </c>
+      <c r="L24" s="78">
+        <v>1</v>
+      </c>
+      <c r="M24" s="19" t="s">
         <v>291</v>
-      </c>
-      <c r="L24" s="78">
-        <v>1</v>
-      </c>
-      <c r="M24" s="19">
-        <v>0</v>
       </c>
       <c r="N24" s="19">
         <v>0</v>
@@ -7840,17 +7840,17 @@
       <c r="J25" s="19">
         <v>0</v>
       </c>
-      <c r="K25" s="19" t="s">
+      <c r="K25" s="78">
+        <v>1</v>
+      </c>
+      <c r="L25" s="19">
+        <v>0</v>
+      </c>
+      <c r="M25" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L25" s="19">
-        <v>0</v>
-      </c>
-      <c r="M25" s="19">
-        <v>0</v>
-      </c>
-      <c r="N25" s="78">
-        <v>1</v>
+      <c r="N25" s="19">
+        <v>0</v>
       </c>
       <c r="O25" s="19">
         <v>0</v>
@@ -7905,17 +7905,17 @@
       <c r="J26" s="19">
         <v>0</v>
       </c>
-      <c r="K26" s="19" t="s">
+      <c r="K26" s="78">
+        <v>1</v>
+      </c>
+      <c r="L26" s="19">
+        <v>0</v>
+      </c>
+      <c r="M26" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L26" s="19">
-        <v>0</v>
-      </c>
-      <c r="M26" s="19">
-        <v>0</v>
-      </c>
-      <c r="N26" s="78">
-        <v>1</v>
+      <c r="N26" s="19">
+        <v>0</v>
       </c>
       <c r="O26" s="19">
         <v>0</v>
@@ -7970,17 +7970,17 @@
       <c r="J27" s="19">
         <v>0</v>
       </c>
-      <c r="K27" s="19" t="s">
+      <c r="K27" s="78">
+        <v>1</v>
+      </c>
+      <c r="L27" s="19">
+        <v>0</v>
+      </c>
+      <c r="M27" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L27" s="19">
-        <v>0</v>
-      </c>
-      <c r="M27" s="19">
-        <v>0</v>
-      </c>
-      <c r="N27" s="78">
-        <v>1</v>
+      <c r="N27" s="19">
+        <v>0</v>
       </c>
       <c r="O27" s="19">
         <v>0</v>
@@ -8035,17 +8035,17 @@
       <c r="J28" s="19">
         <v>0</v>
       </c>
-      <c r="K28" s="19" t="s">
+      <c r="K28" s="78">
+        <v>1</v>
+      </c>
+      <c r="L28" s="19">
+        <v>0</v>
+      </c>
+      <c r="M28" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L28" s="19">
-        <v>0</v>
-      </c>
-      <c r="M28" s="19">
-        <v>0</v>
-      </c>
-      <c r="N28" s="78">
-        <v>1</v>
+      <c r="N28" s="19">
+        <v>0</v>
       </c>
       <c r="O28" s="19">
         <v>0</v>
@@ -8100,16 +8100,16 @@
       <c r="J29" s="72">
         <v>1</v>
       </c>
-      <c r="K29" s="19" t="s">
+      <c r="K29" s="78">
+        <v>0</v>
+      </c>
+      <c r="L29" s="78">
+        <v>1</v>
+      </c>
+      <c r="M29" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="L29" s="78">
-        <v>1</v>
-      </c>
-      <c r="M29" s="19">
-        <v>0</v>
-      </c>
-      <c r="N29" s="78">
+      <c r="N29" s="19">
         <v>0</v>
       </c>
       <c r="O29" s="19">
@@ -8165,17 +8165,17 @@
       <c r="J30" s="19">
         <v>0</v>
       </c>
-      <c r="K30" s="19" t="s">
+      <c r="K30" s="78">
+        <v>1</v>
+      </c>
+      <c r="L30" s="19">
+        <v>0</v>
+      </c>
+      <c r="M30" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L30" s="19">
-        <v>0</v>
-      </c>
-      <c r="M30" s="19">
-        <v>0</v>
-      </c>
-      <c r="N30" s="78">
-        <v>1</v>
+      <c r="N30" s="19">
+        <v>0</v>
       </c>
       <c r="O30" s="19">
         <v>0</v>
@@ -8230,17 +8230,17 @@
       <c r="J31" s="19">
         <v>0</v>
       </c>
-      <c r="K31" s="19" t="s">
+      <c r="K31" s="78">
+        <v>1</v>
+      </c>
+      <c r="L31" s="19">
+        <v>0</v>
+      </c>
+      <c r="M31" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L31" s="19">
-        <v>0</v>
-      </c>
-      <c r="M31" s="19">
-        <v>0</v>
-      </c>
-      <c r="N31" s="78">
-        <v>1</v>
+      <c r="N31" s="19">
+        <v>0</v>
       </c>
       <c r="O31" s="19">
         <v>0</v>
@@ -8295,17 +8295,17 @@
       <c r="J32" s="19">
         <v>0</v>
       </c>
-      <c r="K32" s="19" t="s">
+      <c r="K32" s="78">
+        <v>1</v>
+      </c>
+      <c r="L32" s="19">
+        <v>0</v>
+      </c>
+      <c r="M32" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L32" s="19">
-        <v>0</v>
-      </c>
-      <c r="M32" s="19">
-        <v>0</v>
-      </c>
-      <c r="N32" s="78">
-        <v>1</v>
+      <c r="N32" s="19">
+        <v>0</v>
       </c>
       <c r="O32" s="19">
         <v>0</v>
@@ -8360,17 +8360,17 @@
       <c r="J33" s="19">
         <v>0</v>
       </c>
-      <c r="K33" s="19" t="s">
+      <c r="K33" s="78">
+        <v>1</v>
+      </c>
+      <c r="L33" s="19">
+        <v>0</v>
+      </c>
+      <c r="M33" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L33" s="19">
-        <v>0</v>
-      </c>
-      <c r="M33" s="19">
-        <v>0</v>
-      </c>
-      <c r="N33" s="78">
-        <v>1</v>
+      <c r="N33" s="19">
+        <v>0</v>
       </c>
       <c r="O33" s="19">
         <v>0</v>
@@ -8425,17 +8425,17 @@
       <c r="J34" s="72">
         <v>1</v>
       </c>
-      <c r="K34" s="19" t="s">
+      <c r="K34" s="78">
+        <v>2</v>
+      </c>
+      <c r="L34" s="78">
+        <v>1</v>
+      </c>
+      <c r="M34" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="L34" s="78">
-        <v>1</v>
-      </c>
-      <c r="M34" s="19">
-        <v>0</v>
-      </c>
-      <c r="N34" s="78">
-        <v>2</v>
+      <c r="N34" s="19">
+        <v>0</v>
       </c>
       <c r="O34" s="19">
         <v>0</v>
@@ -8490,17 +8490,17 @@
       <c r="J35" s="19">
         <v>0</v>
       </c>
-      <c r="K35" s="19" t="s">
+      <c r="K35" s="78">
+        <v>1</v>
+      </c>
+      <c r="L35" s="19">
+        <v>0</v>
+      </c>
+      <c r="M35" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L35" s="19">
-        <v>0</v>
-      </c>
-      <c r="M35" s="19">
-        <v>0</v>
-      </c>
-      <c r="N35" s="78">
-        <v>1</v>
+      <c r="N35" s="19">
+        <v>0</v>
       </c>
       <c r="O35" s="19">
         <v>0</v>
@@ -8555,17 +8555,17 @@
       <c r="J36" s="19">
         <v>0</v>
       </c>
-      <c r="K36" s="19" t="s">
+      <c r="K36" s="78">
+        <v>1</v>
+      </c>
+      <c r="L36" s="19">
+        <v>0</v>
+      </c>
+      <c r="M36" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L36" s="19">
-        <v>0</v>
-      </c>
-      <c r="M36" s="19">
-        <v>0</v>
-      </c>
-      <c r="N36" s="78">
-        <v>1</v>
+      <c r="N36" s="19">
+        <v>0</v>
       </c>
       <c r="O36" s="19">
         <v>0</v>
@@ -8620,17 +8620,17 @@
       <c r="J37" s="19">
         <v>0</v>
       </c>
-      <c r="K37" s="19" t="s">
+      <c r="K37" s="78">
+        <v>1</v>
+      </c>
+      <c r="L37" s="19">
+        <v>0</v>
+      </c>
+      <c r="M37" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="L37" s="19">
-        <v>0</v>
-      </c>
-      <c r="M37" s="19">
-        <v>0</v>
-      </c>
-      <c r="N37" s="78">
-        <v>1</v>
+      <c r="N37" s="19">
+        <v>0</v>
       </c>
       <c r="O37" s="19">
         <v>0</v>
@@ -8680,19 +8680,19 @@
         <v>0</v>
       </c>
       <c r="I38" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" s="19">
         <v>0</v>
       </c>
-      <c r="K38" s="19" t="s">
+      <c r="K38" s="19">
+        <v>0</v>
+      </c>
+      <c r="L38" s="19">
+        <v>0</v>
+      </c>
+      <c r="M38" s="19" t="s">
         <v>207</v>
-      </c>
-      <c r="L38" s="19">
-        <v>0</v>
-      </c>
-      <c r="M38" s="19">
-        <v>0</v>
       </c>
       <c r="N38" s="19">
         <v>0</v>
@@ -8750,17 +8750,17 @@
       <c r="J39" s="19">
         <v>0</v>
       </c>
-      <c r="K39" s="19" t="s">
+      <c r="K39" s="78">
+        <v>1</v>
+      </c>
+      <c r="L39" s="19">
+        <v>0</v>
+      </c>
+      <c r="M39" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L39" s="19">
-        <v>0</v>
-      </c>
-      <c r="M39" s="19">
-        <v>0</v>
-      </c>
-      <c r="N39" s="78">
-        <v>1</v>
+      <c r="N39" s="19">
+        <v>0</v>
       </c>
       <c r="O39" s="19">
         <v>0</v>
@@ -8815,17 +8815,17 @@
       <c r="J40" s="19">
         <v>0</v>
       </c>
-      <c r="K40" s="19" t="s">
+      <c r="K40" s="78">
+        <v>1</v>
+      </c>
+      <c r="L40" s="19">
+        <v>0</v>
+      </c>
+      <c r="M40" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L40" s="19">
-        <v>0</v>
-      </c>
-      <c r="M40" s="19">
-        <v>0</v>
-      </c>
-      <c r="N40" s="78">
-        <v>1</v>
+      <c r="N40" s="19">
+        <v>0</v>
       </c>
       <c r="O40" s="19">
         <v>0</v>
@@ -8880,17 +8880,17 @@
       <c r="J41" s="19">
         <v>0</v>
       </c>
-      <c r="K41" s="19" t="s">
+      <c r="K41" s="78">
+        <v>1</v>
+      </c>
+      <c r="L41" s="19">
+        <v>0</v>
+      </c>
+      <c r="M41" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L41" s="19">
-        <v>0</v>
-      </c>
-      <c r="M41" s="19">
-        <v>0</v>
-      </c>
-      <c r="N41" s="78">
-        <v>1</v>
+      <c r="N41" s="19">
+        <v>0</v>
       </c>
       <c r="O41" s="19">
         <v>0</v>
@@ -8937,7 +8937,7 @@
         <v>0</v>
       </c>
       <c r="H42" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" s="19">
         <v>0</v>
@@ -8945,17 +8945,17 @@
       <c r="J42" s="19">
         <v>0</v>
       </c>
-      <c r="K42" s="19" t="s">
+      <c r="K42" s="78">
+        <v>2</v>
+      </c>
+      <c r="L42" s="19">
+        <v>0</v>
+      </c>
+      <c r="M42" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="L42" s="19">
-        <v>0</v>
-      </c>
-      <c r="M42" s="19">
-        <v>0</v>
-      </c>
-      <c r="N42" s="78">
-        <v>2</v>
+      <c r="N42" s="19">
+        <v>0</v>
       </c>
       <c r="O42" s="19">
         <v>0</v>
@@ -9010,17 +9010,17 @@
       <c r="J43" s="19">
         <v>0</v>
       </c>
-      <c r="K43" s="19" t="s">
+      <c r="K43" s="78">
+        <v>1</v>
+      </c>
+      <c r="L43" s="19">
+        <v>0</v>
+      </c>
+      <c r="M43" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L43" s="19">
-        <v>0</v>
-      </c>
-      <c r="M43" s="19">
-        <v>0</v>
-      </c>
-      <c r="N43" s="78">
-        <v>1</v>
+      <c r="N43" s="19">
+        <v>0</v>
       </c>
       <c r="O43" s="19">
         <v>0</v>
@@ -9075,17 +9075,17 @@
       <c r="J44" s="19">
         <v>0</v>
       </c>
-      <c r="K44" s="19" t="s">
+      <c r="K44" s="78">
+        <v>1</v>
+      </c>
+      <c r="L44" s="19">
+        <v>0</v>
+      </c>
+      <c r="M44" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L44" s="19">
-        <v>0</v>
-      </c>
-      <c r="M44" s="19">
-        <v>0</v>
-      </c>
-      <c r="N44" s="78">
-        <v>1</v>
+      <c r="N44" s="19">
+        <v>0</v>
       </c>
       <c r="O44" s="19">
         <v>0</v>
@@ -9140,17 +9140,17 @@
       <c r="J45" s="19">
         <v>0</v>
       </c>
-      <c r="K45" s="19" t="s">
+      <c r="K45" s="78">
+        <v>1</v>
+      </c>
+      <c r="L45" s="19">
+        <v>0</v>
+      </c>
+      <c r="M45" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="L45" s="19">
-        <v>0</v>
-      </c>
-      <c r="M45" s="19">
-        <v>0</v>
-      </c>
-      <c r="N45" s="78">
-        <v>1</v>
+      <c r="N45" s="19">
+        <v>0</v>
       </c>
       <c r="O45" s="19">
         <v>0</v>
@@ -9194,7 +9194,7 @@
         <v>0</v>
       </c>
       <c r="G46" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" s="19">
         <v>0</v>
@@ -9205,17 +9205,17 @@
       <c r="J46" s="19">
         <v>0</v>
       </c>
-      <c r="K46" s="19" t="s">
+      <c r="K46" s="78">
+        <v>2</v>
+      </c>
+      <c r="L46" s="19">
+        <v>0</v>
+      </c>
+      <c r="M46" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="L46" s="19">
-        <v>0</v>
-      </c>
-      <c r="M46" s="19">
-        <v>0</v>
-      </c>
-      <c r="N46" s="78">
-        <v>2</v>
+      <c r="N46" s="19">
+        <v>0</v>
       </c>
       <c r="O46" s="19">
         <v>0</v>
@@ -9241,10 +9241,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="P2:R2"/>
     <mergeCell ref="S2:U2"/>
-    <mergeCell ref="K2:O2"/>
     <mergeCell ref="D2:I2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="K2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>